<commit_message>
Iteration 1 of scheduled wash planner_4,buggy
</commit_message>
<xml_diff>
--- a/ProductionPlannerBILAL/test.xlsx
+++ b/ProductionPlannerBILAL/test.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://noumihub-my.sharepoint.com/personal/bilal_anwar_noumi_com_au/Documents/Desktop/Testing python/Planning 1/final final wtith wash/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ariro\OneDrive\Documents\Code\Noumi\Noumi\ProductionPlannerBILAL\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="17" documentId="13_ncr:1_{7309C071-E1DD-45F1-8191-DD038D4C0466}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2E103217-5378-41E1-9592-A012E157FE3B}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B96E818D-2626-43C6-883E-85D84E51BBA6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="18">
   <si>
     <t>product name</t>
   </si>
@@ -62,13 +62,31 @@
     <t>First Wash Time</t>
   </si>
   <si>
-    <t>Product A</t>
-  </si>
-  <si>
-    <t>Product B</t>
-  </si>
-  <si>
-    <t>Product C</t>
+    <t>Additional Wash</t>
+  </si>
+  <si>
+    <t>AO Almond Unsweetened 8x1L HC</t>
+  </si>
+  <si>
+    <t>No</t>
+  </si>
+  <si>
+    <t>WW Almond Milk U/S 8x1L</t>
+  </si>
+  <si>
+    <t>MILKLAB Almond Int'l 8x1L</t>
+  </si>
+  <si>
+    <t>MILKLAB Almond 8x1L</t>
+  </si>
+  <si>
+    <t>Aldi I/G Barista Almond 8x1L</t>
+  </si>
+  <si>
+    <t>AO Barista Almond 8x1L</t>
+  </si>
+  <si>
+    <t>MILKLAB Almond 8x1L (Additional batches)</t>
   </si>
 </sst>
 </file>
@@ -100,7 +118,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -123,16 +141,34 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="6">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -435,10 +471,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K4"/>
+  <dimension ref="A1:Q9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+      <selection activeCell="I11" sqref="I11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -452,123 +488,289 @@
     <col min="7" max="7" width="8.7109375" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="7.85546875" customWidth="1"/>
     <col min="9" max="9" width="19.7109375" customWidth="1"/>
+    <col min="10" max="10" width="27" customWidth="1"/>
+    <col min="11" max="11" width="32.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="G1" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="H1" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="I1" s="3" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+      <c r="J1" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="B2">
-        <v>10000</v>
-      </c>
-      <c r="C2">
-        <v>2000</v>
-      </c>
-      <c r="D2">
-        <v>0.5</v>
-      </c>
-      <c r="E2">
-        <v>0</v>
-      </c>
-      <c r="F2" s="2">
-        <v>45919.833333333336</v>
-      </c>
-      <c r="G2">
-        <v>300</v>
-      </c>
-      <c r="H2">
-        <v>1440</v>
-      </c>
-      <c r="I2" s="2">
-        <v>45919.3125</v>
-      </c>
-      <c r="K2">
+      <c r="K1" s="1"/>
+    </row>
+    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B2" s="2">
+        <v>55488</v>
+      </c>
+      <c r="C2" s="2">
+        <v>15000</v>
+      </c>
+      <c r="D2" s="2">
+        <v>0.7</v>
+      </c>
+      <c r="E2" s="2">
+        <v>0</v>
+      </c>
+      <c r="F2" s="4">
+        <v>45922.354166666664</v>
+      </c>
+      <c r="G2" s="2">
+        <v>360</v>
+      </c>
+      <c r="H2" s="2">
+        <v>3120</v>
+      </c>
+      <c r="I2" s="4">
+        <v>45921.9375</v>
+      </c>
+      <c r="J2" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="Q2">
         <f>B2/(C2*D2)</f>
-        <v>10</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>10</v>
-      </c>
-      <c r="B3">
+        <v>5.2845714285714287</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B3" s="2">
+        <v>90744</v>
+      </c>
+      <c r="C3" s="2">
         <v>15000</v>
       </c>
-      <c r="C3">
-        <v>2500</v>
-      </c>
-      <c r="D3">
-        <v>0.5</v>
-      </c>
-      <c r="E3">
-        <v>45</v>
-      </c>
-      <c r="G3">
-        <v>300</v>
-      </c>
-      <c r="H3">
-        <v>1440</v>
-      </c>
-      <c r="K3">
-        <f t="shared" ref="K3:K4" si="0">B3/(C3*D3)</f>
-        <v>12</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+      <c r="D3" s="2">
+        <v>0.7</v>
+      </c>
+      <c r="E3" s="2">
+        <v>40</v>
+      </c>
+      <c r="F3" s="2"/>
+      <c r="G3" s="2">
+        <v>0</v>
+      </c>
+      <c r="H3" s="2">
+        <v>0</v>
+      </c>
+      <c r="I3" s="2"/>
+      <c r="J3" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="B4">
-        <v>12000</v>
-      </c>
-      <c r="C4">
-        <v>2200</v>
-      </c>
-      <c r="D4">
-        <v>0.5</v>
-      </c>
-      <c r="E4">
-        <v>30</v>
-      </c>
-      <c r="G4">
-        <v>300</v>
-      </c>
-      <c r="H4">
-        <v>1440</v>
-      </c>
-      <c r="K4">
-        <f t="shared" si="0"/>
-        <v>10.909090909090908</v>
-      </c>
+      <c r="K3" s="2"/>
+      <c r="Q3">
+        <f>B3/(C3*D3)</f>
+        <v>8.6422857142857143</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B4" s="2">
+        <v>180000</v>
+      </c>
+      <c r="C4" s="2">
+        <v>15000</v>
+      </c>
+      <c r="D4" s="2">
+        <v>0.85</v>
+      </c>
+      <c r="E4" s="2">
+        <v>220</v>
+      </c>
+      <c r="F4" s="2"/>
+      <c r="G4" s="2">
+        <v>0</v>
+      </c>
+      <c r="H4" s="2">
+        <v>0</v>
+      </c>
+      <c r="I4" s="2"/>
+      <c r="J4" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="K4" s="2"/>
+      <c r="Q4">
+        <f>B4/(C4*D4)</f>
+        <v>14.117647058823529</v>
+      </c>
+    </row>
+    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B5" s="2">
+        <v>364512</v>
+      </c>
+      <c r="C5" s="2">
+        <v>15000</v>
+      </c>
+      <c r="D5" s="2">
+        <v>0.85</v>
+      </c>
+      <c r="E5" s="2">
+        <v>40</v>
+      </c>
+      <c r="F5" s="2"/>
+      <c r="G5" s="2">
+        <v>0</v>
+      </c>
+      <c r="H5" s="2">
+        <v>0</v>
+      </c>
+      <c r="I5" s="2"/>
+      <c r="J5" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="K5" s="2"/>
+    </row>
+    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B6" s="2">
+        <v>151880</v>
+      </c>
+      <c r="C6" s="2">
+        <v>15000</v>
+      </c>
+      <c r="D6" s="2">
+        <v>0.85</v>
+      </c>
+      <c r="E6" s="2">
+        <v>40</v>
+      </c>
+      <c r="F6" s="2"/>
+      <c r="G6" s="2">
+        <v>0</v>
+      </c>
+      <c r="H6" s="2">
+        <v>0</v>
+      </c>
+      <c r="I6" s="2"/>
+      <c r="J6" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="K6" s="2"/>
+    </row>
+    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A7" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B7" s="2">
+        <v>60000</v>
+      </c>
+      <c r="C7" s="2">
+        <v>15000</v>
+      </c>
+      <c r="D7" s="2">
+        <v>0.85</v>
+      </c>
+      <c r="E7" s="2">
+        <v>220</v>
+      </c>
+      <c r="F7" s="2"/>
+      <c r="G7" s="2">
+        <v>0</v>
+      </c>
+      <c r="H7" s="2">
+        <v>0</v>
+      </c>
+      <c r="I7" s="2"/>
+      <c r="J7" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="K7" s="2"/>
+    </row>
+    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A8" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B8" s="2">
+        <v>91128</v>
+      </c>
+      <c r="C8" s="2">
+        <v>15000</v>
+      </c>
+      <c r="D8" s="2">
+        <v>0.85</v>
+      </c>
+      <c r="E8" s="2">
+        <v>40</v>
+      </c>
+      <c r="F8" s="2"/>
+      <c r="G8" s="2">
+        <v>0</v>
+      </c>
+      <c r="H8" s="2">
+        <v>0</v>
+      </c>
+      <c r="I8" s="2"/>
+      <c r="J8" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="K8" s="2"/>
+    </row>
+    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A9" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B9" s="2">
+        <v>121184</v>
+      </c>
+      <c r="C9" s="2">
+        <v>15000</v>
+      </c>
+      <c r="D9" s="2">
+        <v>0.85</v>
+      </c>
+      <c r="E9" s="2">
+        <v>40</v>
+      </c>
+      <c r="F9" s="2"/>
+      <c r="G9" s="2">
+        <v>0</v>
+      </c>
+      <c r="H9" s="2">
+        <v>0</v>
+      </c>
+      <c r="I9" s="2"/>
+      <c r="J9" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="K9" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>